<commit_message>
2nd submission. Revised based on comments.
</commit_message>
<xml_diff>
--- a/projects/capstone/deep_learning/misc_files/experiment_results.xlsx
+++ b/projects/capstone/deep_learning/misc_files/experiment_results.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bencxs\Desktop\cnn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bencxs\workspace\MLND_2\Project\machine-learning\projects\capstone\deep_learning\misc_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Model Refinements" sheetId="2" r:id="rId1"/>
+    <sheet name="Confusion Mat" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="111">
   <si>
     <t>Learning Rate</t>
   </si>
@@ -322,12 +323,51 @@
   </si>
   <si>
     <t>CNN_model_multi_tmp5.ckpt</t>
+  </si>
+  <si>
+    <t>slot 1</t>
+  </si>
+  <si>
+    <t>slot 2</t>
+  </si>
+  <si>
+    <t>slot 3</t>
+  </si>
+  <si>
+    <t>slot 4</t>
+  </si>
+  <si>
+    <t>slot 5</t>
+  </si>
+  <si>
+    <t>AVG</t>
+  </si>
+  <si>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>FN</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>F1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -371,11 +411,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -659,7 +700,7 @@
   <dimension ref="A1:X69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2709,10 +2750,631 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:H35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4">
+        <v>12066</v>
+      </c>
+      <c r="D4">
+        <v>11951</v>
+      </c>
+      <c r="E4">
+        <v>12617</v>
+      </c>
+      <c r="F4">
+        <v>13022</v>
+      </c>
+      <c r="G4">
+        <v>13066</v>
+      </c>
+      <c r="H4">
+        <f>SUM(C4:G4)/5</f>
+        <v>12544.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5">
+        <v>1002</v>
+      </c>
+      <c r="D5">
+        <v>1117</v>
+      </c>
+      <c r="E5">
+        <v>451</v>
+      </c>
+      <c r="F5">
+        <v>46</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:H9" si="0">SUM(C5:G5)/5</f>
+        <v>523.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6">
+        <v>1002</v>
+      </c>
+      <c r="D6">
+        <v>1857</v>
+      </c>
+      <c r="E6">
+        <v>451</v>
+      </c>
+      <c r="F6">
+        <v>46</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>671.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="4">
+        <f>C4/(C4+C5)</f>
+        <v>0.92332415059687789</v>
+      </c>
+      <c r="D7" s="4">
+        <f t="shared" ref="D7:G7" si="1">D4/(D4+D5)</f>
+        <v>0.9145240281603918</v>
+      </c>
+      <c r="E7" s="4">
+        <f t="shared" si="1"/>
+        <v>0.96548821548821551</v>
+      </c>
+      <c r="F7" s="4">
+        <f t="shared" si="1"/>
+        <v>0.99647995102540554</v>
+      </c>
+      <c r="G7" s="4">
+        <f t="shared" si="1"/>
+        <v>0.99984695439240889</v>
+      </c>
+      <c r="H7" s="4">
+        <f t="shared" si="0"/>
+        <v>0.95993265993265986</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="4">
+        <f>C4/(C4+C6)</f>
+        <v>0.92332415059687789</v>
+      </c>
+      <c r="D8" s="4">
+        <f t="shared" ref="D8:G8" si="2">D4/(D4+D6)</f>
+        <v>0.86551274623406715</v>
+      </c>
+      <c r="E8" s="4">
+        <f t="shared" si="2"/>
+        <v>0.96548821548821551</v>
+      </c>
+      <c r="F8" s="4">
+        <f t="shared" si="2"/>
+        <v>0.99647995102540554</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="2"/>
+        <v>0.99984695439240889</v>
+      </c>
+      <c r="H8" s="4">
+        <f t="shared" si="0"/>
+        <v>0.95013040354739497</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="4">
+        <f>2*(C7*C8)/(C7+C8)</f>
+        <v>0.92332415059687789</v>
+      </c>
+      <c r="D9" s="4">
+        <f t="shared" ref="D9:G9" si="3">2*(D7*D8)/(D7+D8)</f>
+        <v>0.88934365232921564</v>
+      </c>
+      <c r="E9" s="4">
+        <f t="shared" si="3"/>
+        <v>0.96548821548821551</v>
+      </c>
+      <c r="F9" s="4">
+        <f t="shared" si="3"/>
+        <v>0.99647995102540554</v>
+      </c>
+      <c r="G9" s="4">
+        <f t="shared" si="3"/>
+        <v>0.99984695439240889</v>
+      </c>
+      <c r="H9" s="4">
+        <f t="shared" si="0"/>
+        <v>0.95489658476642458</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>17</v>
+      </c>
+      <c r="D11">
+        <v>122</v>
+      </c>
+      <c r="E11">
+        <v>37</v>
+      </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>214</v>
+      </c>
+      <c r="D12">
+        <v>120</v>
+      </c>
+      <c r="E12">
+        <v>63</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>78</v>
+      </c>
+      <c r="D13">
+        <v>63</v>
+      </c>
+      <c r="E13">
+        <v>26</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>128</v>
+      </c>
+      <c r="D14">
+        <v>98</v>
+      </c>
+      <c r="E14">
+        <v>37</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>66</v>
+      </c>
+      <c r="D15">
+        <v>51</v>
+      </c>
+      <c r="E15">
+        <v>26</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>102</v>
+      </c>
+      <c r="D16">
+        <v>114</v>
+      </c>
+      <c r="E16">
+        <v>46</v>
+      </c>
+      <c r="F16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>143</v>
+      </c>
+      <c r="D17">
+        <v>103</v>
+      </c>
+      <c r="E17">
+        <v>47</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>62</v>
+      </c>
+      <c r="D18">
+        <v>75</v>
+      </c>
+      <c r="E18">
+        <v>20</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>99</v>
+      </c>
+      <c r="D19">
+        <v>106</v>
+      </c>
+      <c r="E19">
+        <v>19</v>
+      </c>
+      <c r="F19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>93</v>
+      </c>
+      <c r="D20">
+        <v>90</v>
+      </c>
+      <c r="E20">
+        <v>39</v>
+      </c>
+      <c r="F20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>10</v>
+      </c>
+      <c r="D21">
+        <v>175</v>
+      </c>
+      <c r="E21">
+        <v>91</v>
+      </c>
+      <c r="F21">
+        <v>15</v>
+      </c>
+      <c r="G21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <f>SUM(C11:C20)</f>
+        <v>1002</v>
+      </c>
+      <c r="D22">
+        <f>SUM(D11:D21)</f>
+        <v>1117</v>
+      </c>
+      <c r="E22">
+        <f>SUM(E11:E21)</f>
+        <v>451</v>
+      </c>
+      <c r="F22">
+        <f>SUM(F11:F21)</f>
+        <v>46</v>
+      </c>
+      <c r="G22">
+        <f>SUM(G11:G21)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>107</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>11</v>
+      </c>
+      <c r="D24">
+        <v>94</v>
+      </c>
+      <c r="E24">
+        <v>34</v>
+      </c>
+      <c r="F24">
+        <v>5</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>136</v>
+      </c>
+      <c r="D25">
+        <v>88</v>
+      </c>
+      <c r="E25">
+        <v>23</v>
+      </c>
+      <c r="F25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>205</v>
+      </c>
+      <c r="D26">
+        <v>131</v>
+      </c>
+      <c r="E26">
+        <v>32</v>
+      </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>196</v>
+      </c>
+      <c r="D27">
+        <v>151</v>
+      </c>
+      <c r="E27">
+        <v>39</v>
+      </c>
+      <c r="F27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28">
+        <v>79</v>
+      </c>
+      <c r="D28">
+        <v>96</v>
+      </c>
+      <c r="E28">
+        <v>22</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <v>69</v>
+      </c>
+      <c r="D29">
+        <v>96</v>
+      </c>
+      <c r="E29">
+        <v>29</v>
+      </c>
+      <c r="F29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>6</v>
+      </c>
+      <c r="C30">
+        <v>79</v>
+      </c>
+      <c r="D30">
+        <v>102</v>
+      </c>
+      <c r="E30">
+        <v>22</v>
+      </c>
+      <c r="F30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>7</v>
+      </c>
+      <c r="C31">
+        <v>73</v>
+      </c>
+      <c r="D31">
+        <v>60</v>
+      </c>
+      <c r="E31">
+        <v>19</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>8</v>
+      </c>
+      <c r="C32">
+        <v>109</v>
+      </c>
+      <c r="D32">
+        <v>140</v>
+      </c>
+      <c r="E32">
+        <v>45</v>
+      </c>
+      <c r="F32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>9</v>
+      </c>
+      <c r="C33">
+        <v>45</v>
+      </c>
+      <c r="D33">
+        <v>848</v>
+      </c>
+      <c r="E33">
+        <v>32</v>
+      </c>
+      <c r="F33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>10</v>
+      </c>
+      <c r="D34">
+        <v>51</v>
+      </c>
+      <c r="E34">
+        <v>154</v>
+      </c>
+      <c r="F34">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <f>SUM(C24:C33)</f>
+        <v>1002</v>
+      </c>
+      <c r="D35">
+        <f>SUM(D24:D34)</f>
+        <v>1857</v>
+      </c>
+      <c r="E35">
+        <f>SUM(E24:E34)</f>
+        <v>451</v>
+      </c>
+      <c r="F35">
+        <f>SUM(F24:F34)</f>
+        <v>46</v>
+      </c>
+      <c r="G35">
+        <f>SUM(G24:G34)</f>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L57"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>